<commit_message>
Flow Com Saidas(Versao Com Ligeiros Desvios)
</commit_message>
<xml_diff>
--- a/NetData14Bus.xlsx
+++ b/NetData14Bus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinib\Documents\FlowJulio\FPPJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8EE938-2165-4694-A6C4-2572A0F0CB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E3BA1B-60A4-49E6-9537-1B853C27CBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="624" windowWidth="22992" windowHeight="11616" xr2:uid="{576D71CE-C7B3-4906-A030-D8503D98A23B}"/>
+    <workbookView xWindow="0" yWindow="744" windowWidth="22992" windowHeight="11616" xr2:uid="{576D71CE-C7B3-4906-A030-D8503D98A23B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>Tap</t>
   </si>
   <si>
-    <t>C</t>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -401,15 +401,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5861A435-5DD3-4E2E-9D7B-DD3A0ECB4E84}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,14 +425,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -449,13 +449,13 @@
         <v>5.917E-2</v>
       </c>
       <c r="F2" s="2">
-        <v>18.939393939393941</v>
+        <v>5.2799999999999993E-2</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -472,13 +472,14 @@
         <v>0.22303999999999999</v>
       </c>
       <c r="F3" s="2">
-        <v>20.325203252032519</v>
+        <v>4.9200000000000001E-2</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -495,13 +496,14 @@
         <v>0.19797000000000001</v>
       </c>
       <c r="F4" s="2">
-        <v>22.831050228310502</v>
+        <v>4.3799999999999999E-2</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -518,13 +520,14 @@
         <v>0.17632</v>
       </c>
       <c r="F5" s="2">
-        <v>26.737967914438499</v>
+        <v>3.7400000000000003E-2</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -541,13 +544,14 @@
         <v>0.17388000000000001</v>
       </c>
       <c r="F6" s="2">
-        <v>29.411764705882351</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -564,13 +568,14 @@
         <v>0.17102999999999999</v>
       </c>
       <c r="F7" s="2">
-        <v>28.901734104046245</v>
+        <v>3.4599999999999999E-2</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -587,13 +592,14 @@
         <v>4.2110000000000002E-2</v>
       </c>
       <c r="F8" s="2">
-        <v>78.125</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -616,7 +622,7 @@
         <v>0.97799999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -639,7 +645,7 @@
         <v>0.96899999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -662,7 +668,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -685,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -708,7 +714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -731,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -754,7 +760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>